<commit_message>
fixed modularization and bootstrap prepared
</commit_message>
<xml_diff>
--- a/user example.xlsx
+++ b/user example.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="164011"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="2400" windowWidth="22260" windowHeight="12645"/>
+    <workbookView xWindow="0" yWindow="6000" windowWidth="22260" windowHeight="12645"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -19,10 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="6">
-  <si>
-    <t>NIS</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="6">
   <si>
     <t>password</t>
   </si>
@@ -33,10 +30,13 @@
     <t>is_active</t>
   </si>
   <si>
+    <t>username</t>
+  </si>
+  <si>
     <t>walisantri123</t>
   </si>
   <si>
-    <t>siswa</t>
+    <t>wali</t>
   </si>
 </sst>
 </file>
@@ -354,35 +354,36 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D3"/>
+  <dimension ref="A1:D2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B3" sqref="B3"/>
+      <selection activeCell="F4" sqref="F4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="4" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="11.42578125" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="12.7109375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="10.42578125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
+        <v>3</v>
+      </c>
+      <c r="B1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" t="s">
+      <c r="C1" t="s">
         <v>1</v>
       </c>
-      <c r="C1" t="s">
+      <c r="D1" t="s">
         <v>2</v>
-      </c>
-      <c r="D1" t="s">
-        <v>3</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2">
-        <v>123</v>
+        <v>888</v>
       </c>
       <c r="B2" t="s">
         <v>4</v>
@@ -391,20 +392,6 @@
         <v>5</v>
       </c>
       <c r="D2" t="b">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A3">
-        <v>999</v>
-      </c>
-      <c r="B3" t="s">
-        <v>4</v>
-      </c>
-      <c r="C3" t="s">
-        <v>5</v>
-      </c>
-      <c r="D3" t="b">
         <v>1</v>
       </c>
     </row>

</xml_diff>